<commit_message>
cleaned up some work
</commit_message>
<xml_diff>
--- a/dissertation/projectDocs/#ganttChart.xlsx
+++ b/dissertation/projectDocs/#ganttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\uniIndividualProject\individualProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\uniWork\dissertation\projectDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4093BB0C-82FC-497E-8330-AA676FF6E6F6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5172632-715F-4B6F-9A05-6845F798C57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12624" xr2:uid="{9C941148-3515-48F7-9C2B-54F1A7D67116}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9C941148-3515-48F7-9C2B-54F1A7D67116}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -564,20 +566,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A651E6D-E2CE-4812-B02C-4F4B66A8CE2B}">
-  <dimension ref="A1:AD24"/>
+  <dimension ref="A1:AG24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="29" width="12.109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="10.77734375" style="11"/>
+    <col min="2" max="33" width="12.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="10.77734375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="32.4" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -610,7 +612,7 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:30" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
@@ -643,7 +645,7 @@
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="4" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -677,7 +679,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="12"/>
     </row>
-    <row r="5" spans="1:30" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -792,8 +794,24 @@
         <f t="shared" si="0"/>
         <v>43922</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="AD5" s="5">
+        <f t="shared" ref="AD5" si="1">DATE(YEAR(AC5),MONTH(AC5),DAY(AC5)+7)</f>
+        <v>43929</v>
+      </c>
+      <c r="AE5" s="5">
+        <f t="shared" ref="AE5" si="2">DATE(YEAR(AD5),MONTH(AD5),DAY(AD5)+7)</f>
+        <v>43936</v>
+      </c>
+      <c r="AF5" s="5">
+        <f t="shared" ref="AF5:AG5" si="3">DATE(YEAR(AE5),MONTH(AE5),DAY(AE5)+7)</f>
+        <v>43943</v>
+      </c>
+      <c r="AG5" s="5">
+        <f t="shared" si="3"/>
+        <v>43950</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -828,7 +846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -838,7 +856,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -852,19 +870,19 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:30" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
@@ -873,7 +891,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -883,15 +901,16 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -900,8 +919,11 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+    </row>
+    <row r="15" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
@@ -912,7 +934,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:30" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
@@ -920,15 +942,17 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-    </row>
-    <row r="18" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>13</v>
       </c>
@@ -939,7 +963,7 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>23</v>
       </c>
@@ -947,7 +971,7 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>14</v>
       </c>
@@ -958,7 +982,7 @@
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
     </row>
-    <row r="21" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
@@ -977,24 +1001,34 @@
       <c r="Z21" s="10"/>
       <c r="AA21" s="7"/>
     </row>
-    <row r="22" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="AB22" s="7"/>
       <c r="AC22" s="7"/>
-    </row>
-    <row r="23" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="AD22" s="7"/>
+      <c r="AE22" s="7"/>
+    </row>
+    <row r="23" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>15</v>
       </c>
       <c r="AC23" s="7"/>
-    </row>
-    <row r="24" spans="1:29" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
+      <c r="AD23" s="7"/>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+    </row>
+    <row r="24" spans="1:33" s="8" customFormat="1" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>